<commit_message>
modified:   NBA2324.xlsx modified:   completed_games_with_predictions.xlsx modified:   future.xlsx modified:   nba_forecast.ipynb
</commit_message>
<xml_diff>
--- a/NBA2324.xlsx
+++ b/NBA2324.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkdb\OneDrive\Desktop\NBA Projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B00E779-036C-4407-AB98-1285A1B4CB99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BDA231-6CF2-44DF-A92D-F2B2E25C34FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3729" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3777" uniqueCount="74">
   <si>
     <t>Attend.</t>
   </si>
@@ -302,12 +302,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,7 +589,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I621"/>
+  <dimension ref="A1:I629"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -18613,6 +18614,238 @@
         <v>2</v>
       </c>
     </row>
+    <row r="622" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A622" t="s">
+        <v>45</v>
+      </c>
+      <c r="B622" s="3">
+        <v>141</v>
+      </c>
+      <c r="C622" t="s">
+        <v>20</v>
+      </c>
+      <c r="D622" s="3">
+        <v>135</v>
+      </c>
+      <c r="E622" t="s">
+        <v>67</v>
+      </c>
+      <c r="F622">
+        <v>17832</v>
+      </c>
+      <c r="G622" t="s">
+        <v>54</v>
+      </c>
+      <c r="H622" t="s">
+        <v>45</v>
+      </c>
+      <c r="I622" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="623" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A623" t="s">
+        <v>44</v>
+      </c>
+      <c r="B623" s="3">
+        <v>97</v>
+      </c>
+      <c r="C623" t="s">
+        <v>18</v>
+      </c>
+      <c r="D623" s="3">
+        <v>89</v>
+      </c>
+      <c r="E623" t="s">
+        <v>67</v>
+      </c>
+      <c r="F623">
+        <v>17832</v>
+      </c>
+      <c r="G623" t="s">
+        <v>19</v>
+      </c>
+      <c r="H623" t="s">
+        <v>44</v>
+      </c>
+      <c r="I623" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="624" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A624" t="s">
+        <v>39</v>
+      </c>
+      <c r="B624" s="3">
+        <v>131</v>
+      </c>
+      <c r="C624" t="s">
+        <v>14</v>
+      </c>
+      <c r="D624" s="3">
+        <v>127</v>
+      </c>
+      <c r="E624" t="s">
+        <v>67</v>
+      </c>
+      <c r="F624">
+        <v>17832</v>
+      </c>
+      <c r="G624" t="s">
+        <v>55</v>
+      </c>
+      <c r="H624" t="s">
+        <v>39</v>
+      </c>
+      <c r="I624" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="625" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A625" t="s">
+        <v>26</v>
+      </c>
+      <c r="B625" s="3">
+        <v>116</v>
+      </c>
+      <c r="C625" t="s">
+        <v>17</v>
+      </c>
+      <c r="D625" s="3">
+        <v>95</v>
+      </c>
+      <c r="E625" t="s">
+        <v>67</v>
+      </c>
+      <c r="F625">
+        <v>17832</v>
+      </c>
+      <c r="G625" t="s">
+        <v>47</v>
+      </c>
+      <c r="H625" t="s">
+        <v>26</v>
+      </c>
+      <c r="I625" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="626" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A626" t="s">
+        <v>24</v>
+      </c>
+      <c r="B626" s="3">
+        <v>100</v>
+      </c>
+      <c r="C626" t="s">
+        <v>12</v>
+      </c>
+      <c r="D626" s="3">
+        <v>126</v>
+      </c>
+      <c r="E626" t="s">
+        <v>67</v>
+      </c>
+      <c r="F626">
+        <v>17832</v>
+      </c>
+      <c r="G626" t="s">
+        <v>13</v>
+      </c>
+      <c r="H626" t="s">
+        <v>12</v>
+      </c>
+      <c r="I626" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="627" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A627" t="s">
+        <v>30</v>
+      </c>
+      <c r="B627" s="3">
+        <v>96</v>
+      </c>
+      <c r="C627" t="s">
+        <v>33</v>
+      </c>
+      <c r="D627" s="3">
+        <v>125</v>
+      </c>
+      <c r="E627" t="s">
+        <v>67</v>
+      </c>
+      <c r="F627">
+        <v>17832</v>
+      </c>
+      <c r="G627" t="s">
+        <v>34</v>
+      </c>
+      <c r="H627" t="s">
+        <v>33</v>
+      </c>
+      <c r="I627" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="628" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A628" t="s">
+        <v>36</v>
+      </c>
+      <c r="B628" s="3">
+        <v>126</v>
+      </c>
+      <c r="C628" t="s">
+        <v>8</v>
+      </c>
+      <c r="D628" s="3">
+        <v>127</v>
+      </c>
+      <c r="E628" t="s">
+        <v>67</v>
+      </c>
+      <c r="F628">
+        <v>17832</v>
+      </c>
+      <c r="G628" t="s">
+        <v>60</v>
+      </c>
+      <c r="H628" t="s">
+        <v>8</v>
+      </c>
+      <c r="I628" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="629" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A629" t="s">
+        <v>32</v>
+      </c>
+      <c r="B629" s="3">
+        <v>102</v>
+      </c>
+      <c r="C629" t="s">
+        <v>23</v>
+      </c>
+      <c r="D629" s="3">
+        <v>97</v>
+      </c>
+      <c r="E629" t="s">
+        <v>67</v>
+      </c>
+      <c r="F629">
+        <v>17832</v>
+      </c>
+      <c r="G629" t="s">
+        <v>57</v>
+      </c>
+      <c r="H629" t="s">
+        <v>32</v>
+      </c>
+      <c r="I629" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified:   NBA2324.xlsx modified:   future.xlsx modified:   nba_forecast.ipynb
</commit_message>
<xml_diff>
--- a/NBA2324.xlsx
+++ b/NBA2324.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkdb\OneDrive\Desktop\NBA Projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BDA231-6CF2-44DF-A92D-F2B2E25C34FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DCAFE5-0CAE-4A9F-A591-2F1357824763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3777" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3813" uniqueCount="74">
   <si>
     <t>Attend.</t>
   </si>
@@ -589,9 +589,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I629"/>
+  <dimension ref="A1:I635"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A602" workbookViewId="0">
+      <selection activeCell="A634" sqref="A634"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -18846,6 +18848,180 @@
         <v>23</v>
       </c>
     </row>
+    <row r="630" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A630" t="s">
+        <v>27</v>
+      </c>
+      <c r="B630" s="3">
+        <v>114</v>
+      </c>
+      <c r="C630" t="s">
+        <v>42</v>
+      </c>
+      <c r="D630" s="3">
+        <v>125</v>
+      </c>
+      <c r="E630" t="s">
+        <v>67</v>
+      </c>
+      <c r="F630">
+        <v>17832</v>
+      </c>
+      <c r="G630" t="s">
+        <v>43</v>
+      </c>
+      <c r="H630" t="s">
+        <v>42</v>
+      </c>
+      <c r="I630" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="631" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A631" t="s">
+        <v>21</v>
+      </c>
+      <c r="B631" s="3">
+        <v>87</v>
+      </c>
+      <c r="C631" t="s">
+        <v>9</v>
+      </c>
+      <c r="D631" s="3">
+        <v>105</v>
+      </c>
+      <c r="E631" t="s">
+        <v>67</v>
+      </c>
+      <c r="F631">
+        <v>17832</v>
+      </c>
+      <c r="G631" t="s">
+        <v>10</v>
+      </c>
+      <c r="H631" t="s">
+        <v>9</v>
+      </c>
+      <c r="I631" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="632" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A632" t="s">
+        <v>3</v>
+      </c>
+      <c r="B632" s="3">
+        <v>113</v>
+      </c>
+      <c r="C632" t="s">
+        <v>14</v>
+      </c>
+      <c r="D632" s="3">
+        <v>104</v>
+      </c>
+      <c r="E632" t="s">
+        <v>67</v>
+      </c>
+      <c r="F632">
+        <v>17832</v>
+      </c>
+      <c r="G632" t="s">
+        <v>55</v>
+      </c>
+      <c r="H632" t="s">
+        <v>3</v>
+      </c>
+      <c r="I632" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="633" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A633" t="s">
+        <v>11</v>
+      </c>
+      <c r="B633" s="3">
+        <v>116</v>
+      </c>
+      <c r="C633" t="s">
+        <v>8</v>
+      </c>
+      <c r="D633" s="3">
+        <v>107</v>
+      </c>
+      <c r="E633" t="s">
+        <v>67</v>
+      </c>
+      <c r="F633">
+        <v>17832</v>
+      </c>
+      <c r="G633" t="s">
+        <v>60</v>
+      </c>
+      <c r="H633" t="s">
+        <v>11</v>
+      </c>
+      <c r="I633" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="634" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A634" t="s">
+        <v>15</v>
+      </c>
+      <c r="B634" s="3">
+        <v>110</v>
+      </c>
+      <c r="C634" t="s">
+        <v>5</v>
+      </c>
+      <c r="D634" s="3">
+        <v>117</v>
+      </c>
+      <c r="E634" t="s">
+        <v>67</v>
+      </c>
+      <c r="F634">
+        <v>17832</v>
+      </c>
+      <c r="G634" t="s">
+        <v>58</v>
+      </c>
+      <c r="H634" t="s">
+        <v>5</v>
+      </c>
+      <c r="I634" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="635" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A635" t="s">
+        <v>41</v>
+      </c>
+      <c r="B635" s="3">
+        <v>110</v>
+      </c>
+      <c r="C635" t="s">
+        <v>2</v>
+      </c>
+      <c r="D635" s="3">
+        <v>134</v>
+      </c>
+      <c r="E635" t="s">
+        <v>67</v>
+      </c>
+      <c r="F635">
+        <v>17832</v>
+      </c>
+      <c r="G635" t="s">
+        <v>43</v>
+      </c>
+      <c r="H635" t="s">
+        <v>2</v>
+      </c>
+      <c r="I635" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>